<commit_message>
correção 2 desafio 3
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -259,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -301,16 +301,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -457,7 +447,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -586,16 +576,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -986,10 +972,10 @@
   <dimension ref="B2:P30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.55"/>
@@ -1393,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="P14" s="29" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,7 +1749,7 @@
       <c r="F28" s="29" t="n">
         <v>16</v>
       </c>
-      <c r="G28" s="34" t="s">
+      <c r="G28" s="29" t="s">
         <v>73</v>
       </c>
       <c r="H28" s="29" t="n">
@@ -1777,7 +1763,7 @@
       <c r="F29" s="29" t="n">
         <v>17</v>
       </c>
-      <c r="G29" s="34" t="s">
+      <c r="G29" s="29" t="s">
         <v>74</v>
       </c>
       <c r="H29" s="29" t="n">
@@ -1791,7 +1777,7 @@
       <c r="F30" s="29" t="n">
         <v>18</v>
       </c>
-      <c r="G30" s="34" t="s">
+      <c r="G30" s="29" t="s">
         <v>75</v>
       </c>
       <c r="H30" s="29" t="n">

</xml_diff>